<commit_message>
wd removed from 2011 data
</commit_message>
<xml_diff>
--- a/_docs/Data cleaning scripts/ridership/2011/January 2011.xlsx
+++ b/_docs/Data cleaning scripts/ridership/2011/January 2011.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="480" windowWidth="15480" windowHeight="9720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28280"/>
   </bookViews>
   <sheets>
     <sheet name="Weekday OD" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,12 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Sunday OD'!$A:$A</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Weekday OD'!$A:$A</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -218,14 +223,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="mmm\ yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -607,8 +612,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BD63"/>
@@ -621,14 +626,14 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="44" width="7.7109375" style="9" customWidth="1"/>
-    <col min="45" max="45" width="8.7109375" style="11" customWidth="1"/>
-    <col min="46" max="46" width="9.140625" style="11"/>
-    <col min="47" max="48" width="9.140625" style="9"/>
-    <col min="49" max="49" width="8.7109375" style="9" customWidth="1"/>
-    <col min="50" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="44" width="7.6640625" style="9" customWidth="1"/>
+    <col min="45" max="45" width="8.6640625" style="11" customWidth="1"/>
+    <col min="46" max="46" width="8.83203125" style="11"/>
+    <col min="47" max="48" width="8.83203125" style="9"/>
+    <col min="49" max="49" width="8.6640625" style="9" customWidth="1"/>
+    <col min="50" max="16384" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="26.25" customHeight="1">
@@ -7475,14 +7480,19 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="81" fitToWidth="3" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="81" fitToWidth="3" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BD63"/>
@@ -7495,14 +7505,14 @@
       <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="44" width="7.7109375" style="9" customWidth="1"/>
-    <col min="45" max="45" width="8.7109375" style="11" customWidth="1"/>
-    <col min="46" max="46" width="9.140625" style="11"/>
-    <col min="47" max="48" width="9.140625" style="9"/>
-    <col min="49" max="49" width="8.7109375" style="9" customWidth="1"/>
-    <col min="50" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="44" width="7.6640625" style="9" customWidth="1"/>
+    <col min="45" max="45" width="8.6640625" style="11" customWidth="1"/>
+    <col min="46" max="46" width="8.83203125" style="11"/>
+    <col min="47" max="48" width="8.83203125" style="9"/>
+    <col min="49" max="49" width="8.6640625" style="9" customWidth="1"/>
+    <col min="50" max="16384" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="27" customHeight="1">
@@ -14324,14 +14334,19 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="72" fitToWidth="2" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="72" fitToWidth="2" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BD63"/>
@@ -14344,14 +14359,14 @@
       <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="44" width="7.7109375" style="9" customWidth="1"/>
-    <col min="45" max="45" width="8.7109375" style="11" customWidth="1"/>
-    <col min="46" max="46" width="9.140625" style="11"/>
-    <col min="47" max="48" width="9.140625" style="9"/>
-    <col min="49" max="49" width="8.7109375" style="9" customWidth="1"/>
-    <col min="50" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="44" width="7.6640625" style="9" customWidth="1"/>
+    <col min="45" max="45" width="8.6640625" style="11" customWidth="1"/>
+    <col min="46" max="46" width="8.83203125" style="11"/>
+    <col min="47" max="48" width="8.83203125" style="9"/>
+    <col min="49" max="49" width="8.6640625" style="9" customWidth="1"/>
+    <col min="50" max="16384" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="26.25" customHeight="1">
@@ -21173,22 +21188,27 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="72" fitToWidth="2" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="72" fitToWidth="2" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="8.140625" customWidth="1"/>
+    <col min="1" max="10" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -22210,7 +22230,12 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>